<commit_message>
added barcode editor v1 and update master 1P00560048
</commit_message>
<xml_diff>
--- a/master.xlsx
+++ b/master.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\gad-shaily\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4820354-F2EC-4C56-9B76-A971BB96CBD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0198D758-D094-41ED-83DB-42E6DA11C493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$209</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="275">
   <si>
     <t>Wire No.</t>
   </si>
@@ -747,9 +750,6 @@
     <t>SFG00969</t>
   </si>
   <si>
-    <t>UL1569AWG22Orange/Blue(BARE)</t>
-  </si>
-  <si>
     <t>Orange / Blue</t>
   </si>
   <si>
@@ -986,6 +986,18 @@
   </si>
   <si>
     <t>0039000048</t>
+  </si>
+  <si>
+    <t>39000048</t>
+  </si>
+  <si>
+    <t>1P0039000048</t>
+  </si>
+  <si>
+    <t>1P0561349000</t>
+  </si>
+  <si>
+    <t>UL1569AWG22ORANGE/BLUE(BARE)</t>
   </si>
 </sst>
 </file>
@@ -1429,10 +1441,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D101" zoomScale="131" workbookViewId="0">
-      <selection activeCell="G110" sqref="G110"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="131" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1440,8 +1453,10 @@
     <col min="2" max="2" width="41.88671875" customWidth="1"/>
     <col min="3" max="3" width="26.33203125" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
+    <col min="5" max="5" width="25.109375" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" customWidth="1"/>
     <col min="7" max="7" width="32.21875" style="13" customWidth="1"/>
-    <col min="9" max="9" width="31.6640625" customWidth="1"/>
+    <col min="9" max="9" width="31.6640625" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1469,11 +1484,11 @@
       <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -1498,11 +1513,11 @@
       <c r="H2" s="5">
         <v>3</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -1527,11 +1542,11 @@
       <c r="H3" s="5">
         <v>3</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -1556,11 +1571,11 @@
       <c r="H4" s="5">
         <v>3</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
@@ -1585,11 +1600,11 @@
       <c r="H5" s="5">
         <v>3.5</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -1614,11 +1629,11 @@
       <c r="H6" s="5">
         <v>3.5</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>30</v>
       </c>
@@ -1643,11 +1658,11 @@
       <c r="H7" s="5">
         <v>3.5</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
@@ -1672,11 +1687,11 @@
       <c r="H8" s="5">
         <v>3.5</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>35</v>
       </c>
@@ -1701,11 +1716,11 @@
       <c r="H9" s="5">
         <v>3.5</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>35</v>
       </c>
@@ -1728,11 +1743,11 @@
       <c r="H10" s="5">
         <v>5</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>41</v>
       </c>
@@ -1757,11 +1772,11 @@
       <c r="H11" s="5">
         <v>5</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>45</v>
       </c>
@@ -1786,11 +1801,11 @@
       <c r="H12" s="5">
         <v>5</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>49</v>
       </c>
@@ -1815,11 +1830,11 @@
       <c r="H13" s="5">
         <v>3.5</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>54</v>
       </c>
@@ -1844,11 +1859,11 @@
       <c r="H14" s="5">
         <v>3.5</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
@@ -1873,11 +1888,11 @@
       <c r="H15" s="5">
         <v>3.5</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>56</v>
       </c>
@@ -1902,11 +1917,11 @@
       <c r="H16" s="5">
         <v>3.5</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="I16" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>59</v>
       </c>
@@ -1932,11 +1947,11 @@
       <c r="H17" s="5">
         <v>4.5</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>54</v>
       </c>
@@ -1962,11 +1977,11 @@
       <c r="H18" s="5">
         <v>4.5</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="I18" s="11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>64</v>
       </c>
@@ -1991,11 +2006,11 @@
       <c r="H19" s="5">
         <v>5</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="I19" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>49</v>
       </c>
@@ -2021,11 +2036,11 @@
       <c r="H20" s="5">
         <v>5</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="I20" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>68</v>
       </c>
@@ -2050,11 +2065,11 @@
       <c r="H21" s="5">
         <v>3.5</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="I21" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>72</v>
       </c>
@@ -2079,11 +2094,11 @@
       <c r="H22" s="5">
         <v>7</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="I22" s="11" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>75</v>
       </c>
@@ -2108,11 +2123,11 @@
       <c r="H23" s="5">
         <v>7</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="I23" s="11" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>77</v>
       </c>
@@ -2137,11 +2152,11 @@
       <c r="H24" s="5">
         <v>7</v>
       </c>
-      <c r="I24" s="5" t="s">
+      <c r="I24" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>81</v>
       </c>
@@ -2166,11 +2181,11 @@
       <c r="H25" s="5">
         <v>3.5</v>
       </c>
-      <c r="I25" s="5" t="s">
+      <c r="I25" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>84</v>
       </c>
@@ -2196,11 +2211,11 @@
       <c r="H26" s="5">
         <v>4.8</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="I26" s="11" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>68</v>
       </c>
@@ -2226,11 +2241,11 @@
       <c r="H27" s="5">
         <v>4.8</v>
       </c>
-      <c r="I27" s="5" t="s">
+      <c r="I27" s="11" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>54</v>
       </c>
@@ -2255,11 +2270,11 @@
       <c r="H28" s="5">
         <v>3</v>
       </c>
-      <c r="I28" s="5" t="s">
+      <c r="I28" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>64</v>
       </c>
@@ -2284,11 +2299,11 @@
       <c r="H29" s="5">
         <v>7</v>
       </c>
-      <c r="I29" s="5" t="s">
+      <c r="I29" s="11" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>64</v>
       </c>
@@ -2313,11 +2328,11 @@
       <c r="H30" s="5">
         <v>7</v>
       </c>
-      <c r="I30" s="5" t="s">
+      <c r="I30" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>64</v>
       </c>
@@ -2343,11 +2358,11 @@
       <c r="H31" s="5">
         <v>7</v>
       </c>
-      <c r="I31" s="5" t="s">
+      <c r="I31" s="11" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>92</v>
       </c>
@@ -2372,11 +2387,11 @@
       <c r="H32" s="5">
         <v>7</v>
       </c>
-      <c r="I32" s="5" t="s">
+      <c r="I32" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>92</v>
       </c>
@@ -2401,11 +2416,11 @@
       <c r="H33" s="5">
         <v>7</v>
       </c>
-      <c r="I33" s="5" t="s">
+      <c r="I33" s="11" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>92</v>
       </c>
@@ -2430,11 +2445,11 @@
       <c r="H34" s="5">
         <v>7</v>
       </c>
-      <c r="I34" s="5" t="s">
+      <c r="I34" s="11" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>49</v>
       </c>
@@ -2459,11 +2474,11 @@
       <c r="H35" s="5">
         <v>3</v>
       </c>
-      <c r="I35" s="5" t="s">
+      <c r="I35" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>14</v>
       </c>
@@ -2488,11 +2503,11 @@
       <c r="H36" s="5">
         <v>3</v>
       </c>
-      <c r="I36" s="5" t="s">
+      <c r="I36" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>98</v>
       </c>
@@ -2517,11 +2532,11 @@
       <c r="H37" s="5">
         <v>11</v>
       </c>
-      <c r="I37" s="5" t="s">
+      <c r="I37" s="11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>98</v>
       </c>
@@ -2546,11 +2561,11 @@
       <c r="H38" s="5">
         <v>11</v>
       </c>
-      <c r="I38" s="5" t="s">
+      <c r="I38" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>98</v>
       </c>
@@ -2575,11 +2590,11 @@
       <c r="H39" s="5">
         <v>11</v>
       </c>
-      <c r="I39" s="5" t="s">
+      <c r="I39" s="11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>107</v>
       </c>
@@ -2604,11 +2619,11 @@
       <c r="H40" s="5">
         <v>7</v>
       </c>
-      <c r="I40" s="5" t="s">
+      <c r="I40" s="11" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>54</v>
       </c>
@@ -2633,11 +2648,11 @@
       <c r="H41" s="5">
         <v>7</v>
       </c>
-      <c r="I41" s="5" t="s">
+      <c r="I41" s="11" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>14</v>
       </c>
@@ -2662,11 +2677,11 @@
       <c r="H42" s="5">
         <v>3</v>
       </c>
-      <c r="I42" s="5" t="s">
+      <c r="I42" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>112</v>
       </c>
@@ -2691,11 +2706,11 @@
       <c r="H43" s="5">
         <v>3</v>
       </c>
-      <c r="I43" s="5" t="s">
+      <c r="I43" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>115</v>
       </c>
@@ -2720,11 +2735,11 @@
       <c r="H44" s="5">
         <v>7</v>
       </c>
-      <c r="I44" s="5" t="s">
+      <c r="I44" s="11" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>112</v>
       </c>
@@ -2749,11 +2764,11 @@
       <c r="H45" s="5">
         <v>7</v>
       </c>
-      <c r="I45" s="5" t="s">
+      <c r="I45" s="11" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>119</v>
       </c>
@@ -2778,11 +2793,11 @@
       <c r="H46" s="5">
         <v>3</v>
       </c>
-      <c r="I46" s="5" t="s">
+      <c r="I46" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>119</v>
       </c>
@@ -2807,11 +2822,11 @@
       <c r="H47" s="5">
         <v>3</v>
       </c>
-      <c r="I47" s="5" t="s">
+      <c r="I47" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>49</v>
       </c>
@@ -2836,11 +2851,11 @@
       <c r="H48" s="5">
         <v>3</v>
       </c>
-      <c r="I48" s="5" t="s">
+      <c r="I48" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>59</v>
       </c>
@@ -2865,11 +2880,11 @@
       <c r="H49" s="5">
         <v>3.5</v>
       </c>
-      <c r="I49" s="5" t="s">
+      <c r="I49" s="11" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>92</v>
       </c>
@@ -2894,11 +2909,11 @@
       <c r="H50" s="5">
         <v>3.5</v>
       </c>
-      <c r="I50" s="5" t="s">
+      <c r="I50" s="11" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>124</v>
       </c>
@@ -2923,11 +2938,11 @@
       <c r="H51" s="5">
         <v>3.5</v>
       </c>
-      <c r="I51" s="5" t="s">
+      <c r="I51" s="11" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
         <v>81</v>
       </c>
@@ -2952,11 +2967,11 @@
       <c r="H52" s="5">
         <v>3.5</v>
       </c>
-      <c r="I52" s="5" t="s">
+      <c r="I52" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>127</v>
       </c>
@@ -2981,11 +2996,11 @@
       <c r="H53" s="5">
         <v>11</v>
       </c>
-      <c r="I53" s="5" t="s">
+      <c r="I53" s="11" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>133</v>
       </c>
@@ -3010,11 +3025,11 @@
       <c r="H54" s="5">
         <v>5</v>
       </c>
-      <c r="I54" s="5" t="s">
+      <c r="I54" s="11" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>59</v>
       </c>
@@ -3039,11 +3054,11 @@
       <c r="H55" s="5">
         <v>3.5</v>
       </c>
-      <c r="I55" s="5" t="s">
+      <c r="I55" s="11" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
         <v>77</v>
       </c>
@@ -3068,11 +3083,11 @@
       <c r="H56" s="5">
         <v>3</v>
       </c>
-      <c r="I56" s="5">
+      <c r="I56" s="11">
         <v>39000040</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
         <v>127</v>
       </c>
@@ -3097,11 +3112,11 @@
       <c r="H57" s="5">
         <v>11</v>
       </c>
-      <c r="I57" s="5" t="s">
+      <c r="I57" s="11" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
         <v>112</v>
       </c>
@@ -3126,7 +3141,7 @@
       <c r="H58" s="5">
         <v>7</v>
       </c>
-      <c r="I58" s="5" t="s">
+      <c r="I58" s="11" t="s">
         <v>142</v>
       </c>
     </row>
@@ -3155,11 +3170,11 @@
       <c r="H59" s="5">
         <v>7</v>
       </c>
-      <c r="I59" s="5" t="s">
+      <c r="I59" s="11" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
         <v>112</v>
       </c>
@@ -3185,7 +3200,7 @@
       <c r="H60" s="5">
         <v>3</v>
       </c>
-      <c r="I60" s="5">
+      <c r="I60" s="11">
         <v>39000048</v>
       </c>
     </row>
@@ -3215,11 +3230,11 @@
       <c r="H61" s="5">
         <v>2</v>
       </c>
-      <c r="I61" s="5" t="s">
+      <c r="I61" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="s">
         <v>148</v>
       </c>
@@ -3244,11 +3259,11 @@
       <c r="H62" s="5">
         <v>7</v>
       </c>
-      <c r="I62" s="5" t="s">
+      <c r="I62" s="11" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
         <v>145</v>
       </c>
@@ -3274,7 +3289,7 @@
       <c r="H63" s="5">
         <v>3</v>
       </c>
-      <c r="I63" s="5" t="s">
+      <c r="I63" s="11" t="s">
         <v>151</v>
       </c>
     </row>
@@ -3304,11 +3319,11 @@
       <c r="H64" s="5">
         <v>2</v>
       </c>
-      <c r="I64" s="5">
+      <c r="I64" s="11">
         <v>561349000</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
         <v>127</v>
       </c>
@@ -3333,11 +3348,11 @@
       <c r="H65" s="5">
         <v>11</v>
       </c>
-      <c r="I65" s="5" t="s">
+      <c r="I65" s="11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
         <v>68</v>
       </c>
@@ -3363,11 +3378,11 @@
       <c r="H66" s="5">
         <v>3</v>
       </c>
-      <c r="I66" s="5">
+      <c r="I66" s="11">
         <v>39000048</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
         <v>155</v>
       </c>
@@ -3392,11 +3407,11 @@
       <c r="H67" s="5">
         <v>3</v>
       </c>
-      <c r="I67" s="5">
+      <c r="I67" s="11">
         <v>39000048</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
         <v>41</v>
       </c>
@@ -3421,11 +3436,11 @@
       <c r="H68" s="5">
         <v>5</v>
       </c>
-      <c r="I68" s="5" t="s">
+      <c r="I68" s="11" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="s">
         <v>8</v>
       </c>
@@ -3451,11 +3466,11 @@
       <c r="H69" s="5">
         <v>3</v>
       </c>
-      <c r="I69" s="5">
+      <c r="I69" s="11">
         <v>39000048</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
         <v>124</v>
       </c>
@@ -3481,11 +3496,11 @@
       <c r="H70" s="5">
         <v>2</v>
       </c>
-      <c r="I70" s="5" t="s">
+      <c r="I70" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="s">
         <v>8</v>
       </c>
@@ -3510,11 +3525,11 @@
       <c r="H71" s="5">
         <v>2</v>
       </c>
-      <c r="I71" s="5" t="s">
+      <c r="I71" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
         <v>165</v>
       </c>
@@ -3539,11 +3554,11 @@
       <c r="H72" s="5">
         <v>7</v>
       </c>
-      <c r="I72" s="5" t="s">
+      <c r="I72" s="11" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="4" t="s">
         <v>45</v>
       </c>
@@ -3569,11 +3584,11 @@
       <c r="H73" s="5">
         <v>12</v>
       </c>
-      <c r="I73" s="5" t="s">
+      <c r="I73" s="11" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="4" t="s">
         <v>155</v>
       </c>
@@ -3599,11 +3614,11 @@
       <c r="H74" s="5">
         <v>7</v>
       </c>
-      <c r="I74" s="5" t="s">
+      <c r="I74" s="11" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="4" t="s">
         <v>41</v>
       </c>
@@ -3628,11 +3643,11 @@
       <c r="H75" s="5">
         <v>11</v>
       </c>
-      <c r="I75" s="5" t="s">
+      <c r="I75" s="11" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="s">
         <v>72</v>
       </c>
@@ -3657,11 +3672,11 @@
       <c r="H76" s="5">
         <v>7</v>
       </c>
-      <c r="I76" s="5" t="s">
+      <c r="I76" s="11" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="4" t="s">
         <v>35</v>
       </c>
@@ -3686,11 +3701,11 @@
       <c r="H77" s="5">
         <v>11</v>
       </c>
-      <c r="I77" s="5" t="s">
+      <c r="I77" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="4" t="s">
         <v>35</v>
       </c>
@@ -3715,7 +3730,7 @@
       <c r="H78" s="5">
         <v>11</v>
       </c>
-      <c r="I78" s="5" t="s">
+      <c r="I78" s="11" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3744,11 +3759,11 @@
       <c r="H79" s="5">
         <v>7</v>
       </c>
-      <c r="I79" s="5" t="s">
+      <c r="I79" s="11" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="4" t="s">
         <v>84</v>
       </c>
@@ -3773,11 +3788,11 @@
       <c r="H80" s="5">
         <v>3</v>
       </c>
-      <c r="I80" s="5">
+      <c r="I80" s="11">
         <v>39000040</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="4" t="s">
         <v>119</v>
       </c>
@@ -3803,11 +3818,11 @@
       <c r="H81" s="5">
         <v>3</v>
       </c>
-      <c r="I81" s="5">
+      <c r="I81" s="11">
         <v>39000048</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="4" t="s">
         <v>45</v>
       </c>
@@ -3833,11 +3848,11 @@
       <c r="H82" s="5">
         <v>12</v>
       </c>
-      <c r="I82" s="5" t="s">
+      <c r="I82" s="11" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="s">
         <v>180</v>
       </c>
@@ -3863,11 +3878,11 @@
       <c r="H83" s="5">
         <v>12</v>
       </c>
-      <c r="I83" s="5" t="s">
+      <c r="I83" s="11" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="s">
         <v>56</v>
       </c>
@@ -3892,11 +3907,11 @@
       <c r="H84" s="5">
         <v>3.5</v>
       </c>
-      <c r="I84" s="5" t="s">
+      <c r="I84" s="11" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="s">
         <v>49</v>
       </c>
@@ -3921,11 +3936,11 @@
       <c r="H85" s="5">
         <v>3.5</v>
       </c>
-      <c r="I85" s="5" t="s">
+      <c r="I85" s="11" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
         <v>84</v>
       </c>
@@ -3951,7 +3966,7 @@
       <c r="H86" s="5">
         <v>12</v>
       </c>
-      <c r="I86" s="5" t="s">
+      <c r="I86" s="11" t="s">
         <v>179</v>
       </c>
     </row>
@@ -3980,11 +3995,11 @@
       <c r="H87" s="5">
         <v>3</v>
       </c>
-      <c r="I87" s="5">
+      <c r="I87" s="11">
         <v>39000048</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="s">
         <v>64</v>
       </c>
@@ -4009,11 +4024,11 @@
       <c r="H88" s="5">
         <v>7</v>
       </c>
-      <c r="I88" s="5" t="s">
+      <c r="I88" s="11" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="4" t="s">
         <v>92</v>
       </c>
@@ -4038,11 +4053,11 @@
       <c r="H89" s="5">
         <v>7</v>
       </c>
-      <c r="I89" s="5" t="s">
+      <c r="I89" s="11" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="4" t="s">
         <v>54</v>
       </c>
@@ -4068,11 +4083,11 @@
       <c r="H90" s="5">
         <v>7</v>
       </c>
-      <c r="I90" s="5" t="s">
+      <c r="I90" s="11" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="s">
         <v>191</v>
       </c>
@@ -4098,7 +4113,7 @@
       <c r="H91" s="5">
         <v>7</v>
       </c>
-      <c r="I91" s="5" t="s">
+      <c r="I91" s="11" t="s">
         <v>194</v>
       </c>
     </row>
@@ -4127,7 +4142,7 @@
       <c r="H92" s="5">
         <v>7</v>
       </c>
-      <c r="I92" s="5" t="s">
+      <c r="I92" s="11" t="s">
         <v>195</v>
       </c>
     </row>
@@ -4156,11 +4171,11 @@
       <c r="H93" s="5">
         <v>7</v>
       </c>
-      <c r="I93" s="5" t="s">
+      <c r="I93" s="11" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="4" t="s">
         <v>54</v>
       </c>
@@ -4185,11 +4200,11 @@
       <c r="H94" s="5">
         <v>7</v>
       </c>
-      <c r="I94" s="5" t="s">
+      <c r="I94" s="11" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="4" t="s">
         <v>124</v>
       </c>
@@ -4214,7 +4229,7 @@
       <c r="H95" s="5">
         <v>3</v>
       </c>
-      <c r="I95" s="5" t="s">
+      <c r="I95" s="11" t="s">
         <v>91</v>
       </c>
     </row>
@@ -4243,7 +4258,7 @@
       <c r="H96" s="5">
         <v>2</v>
       </c>
-      <c r="I96" s="5">
+      <c r="I96" s="11">
         <v>561349000</v>
       </c>
     </row>
@@ -4272,7 +4287,7 @@
       <c r="H97" s="5">
         <v>2</v>
       </c>
-      <c r="I97" s="5">
+      <c r="I97" s="11">
         <v>561349000</v>
       </c>
     </row>
@@ -4281,13 +4296,13 @@
         <v>198</v>
       </c>
       <c r="B98" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D98" s="8" t="s">
         <v>199</v>
-      </c>
-      <c r="C98" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D98" s="8" t="s">
-        <v>200</v>
       </c>
       <c r="E98" s="8">
         <v>1610</v>
@@ -4295,14 +4310,14 @@
       <c r="F98" s="8">
         <v>3</v>
       </c>
-      <c r="G98" s="12">
-        <v>39000048</v>
+      <c r="G98" s="12" t="s">
+        <v>272</v>
       </c>
       <c r="H98" s="8">
         <v>2</v>
       </c>
-      <c r="I98" s="8">
-        <v>561349000</v>
+      <c r="I98" s="12" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4324,28 +4339,28 @@
       <c r="F99" s="5">
         <v>3</v>
       </c>
-      <c r="G99" s="11">
-        <v>39000048</v>
+      <c r="G99" s="11" t="s">
+        <v>271</v>
       </c>
       <c r="H99" s="5">
         <v>2</v>
       </c>
-      <c r="I99" s="5">
+      <c r="I99" s="11">
         <v>561349000</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B100" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="C100" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D100" s="6" t="s">
         <v>202</v>
-      </c>
-      <c r="C100" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D100" s="6" t="s">
-        <v>203</v>
       </c>
       <c r="E100" s="5">
         <v>960</v>
@@ -4359,11 +4374,11 @@
       <c r="H100" s="5">
         <v>2</v>
       </c>
-      <c r="I100" s="5">
+      <c r="I100" s="11">
         <v>561349000</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="4" t="s">
         <v>119</v>
       </c>
@@ -4388,7 +4403,7 @@
       <c r="H101" s="5">
         <v>2</v>
       </c>
-      <c r="I101" s="5">
+      <c r="I101" s="11">
         <v>561349000</v>
       </c>
     </row>
@@ -4418,11 +4433,11 @@
       <c r="H102" s="5">
         <v>2</v>
       </c>
-      <c r="I102" s="5">
+      <c r="I102" s="11">
         <v>561349000</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="4" t="s">
         <v>59</v>
       </c>
@@ -4448,11 +4463,11 @@
       <c r="H103" s="5">
         <v>3</v>
       </c>
-      <c r="I103" s="5">
+      <c r="I103" s="11">
         <v>39000048</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="4" t="s">
         <v>59</v>
       </c>
@@ -4477,11 +4492,11 @@
       <c r="H104" s="5">
         <v>7</v>
       </c>
-      <c r="I104" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I104" s="11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="4" t="s">
         <v>92</v>
       </c>
@@ -4507,11 +4522,11 @@
       <c r="H105" s="5">
         <v>3</v>
       </c>
-      <c r="I105" s="5">
+      <c r="I105" s="11">
         <v>39000048</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="4" t="s">
         <v>54</v>
       </c>
@@ -4537,11 +4552,11 @@
       <c r="H106" s="5">
         <v>3</v>
       </c>
-      <c r="I106" s="5">
+      <c r="I106" s="11">
         <v>39000048</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="4" t="s">
         <v>124</v>
       </c>
@@ -4567,22 +4582,22 @@
       <c r="H107" s="5">
         <v>3</v>
       </c>
-      <c r="I107" s="5">
+      <c r="I107" s="11">
         <v>39000048</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B108" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="C108" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D108" s="6" t="s">
         <v>206</v>
-      </c>
-      <c r="C108" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D108" s="6" t="s">
-        <v>207</v>
       </c>
       <c r="E108" s="5">
         <v>920</v>
@@ -4596,16 +4611,16 @@
       <c r="H108" s="5">
         <v>5</v>
       </c>
-      <c r="I108" s="5" t="s">
+      <c r="I108" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B109" s="4" t="s">
         <v>208</v>
-      </c>
-      <c r="B109" s="4" t="s">
-        <v>209</v>
       </c>
       <c r="C109" s="5" t="s">
         <v>51</v>
@@ -4626,22 +4641,22 @@
       <c r="H109" s="5">
         <v>5</v>
       </c>
-      <c r="I109" s="5" t="s">
+      <c r="I109" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B110" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="C110" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D110" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="C110" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D110" s="6" t="s">
-        <v>212</v>
       </c>
       <c r="E110" s="5">
         <v>1830</v>
@@ -4650,12 +4665,12 @@
         <v>3</v>
       </c>
       <c r="G110" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H110" s="5">
         <v>2</v>
       </c>
-      <c r="I110" s="5">
+      <c r="I110" s="11">
         <v>561349000</v>
       </c>
     </row>
@@ -4684,7 +4699,7 @@
       <c r="H111" s="5">
         <v>2</v>
       </c>
-      <c r="I111" s="5">
+      <c r="I111" s="11">
         <v>561349000</v>
       </c>
     </row>
@@ -4714,22 +4729,22 @@
       <c r="H112" s="5">
         <v>2</v>
       </c>
-      <c r="I112" s="5">
+      <c r="I112" s="11">
         <v>561349000</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A113" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B113" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="C113" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D113" s="6" t="s">
         <v>214</v>
-      </c>
-      <c r="C113" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D113" s="6" t="s">
-        <v>215</v>
       </c>
       <c r="E113" s="5">
         <v>2410</v>
@@ -4743,11 +4758,11 @@
       <c r="H113" s="5">
         <v>2</v>
       </c>
-      <c r="I113" s="5">
+      <c r="I113" s="11">
         <v>561349000</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A114" s="4" t="s">
         <v>92</v>
       </c>
@@ -4772,11 +4787,11 @@
       <c r="H114" s="5">
         <v>3</v>
       </c>
-      <c r="I114" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I114" s="11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="4" t="s">
         <v>56</v>
       </c>
@@ -4801,11 +4816,11 @@
       <c r="H115" s="5">
         <v>3</v>
       </c>
-      <c r="I115" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I115" s="11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="4" t="s">
         <v>8</v>
       </c>
@@ -4816,7 +4831,7 @@
         <v>51</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E116" s="5">
         <v>960</v>
@@ -4830,11 +4845,11 @@
       <c r="H116" s="5">
         <v>3</v>
       </c>
-      <c r="I116" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I116" s="11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="4" t="s">
         <v>49</v>
       </c>
@@ -4859,22 +4874,22 @@
       <c r="H117" s="5">
         <v>3</v>
       </c>
-      <c r="I117" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I117" s="11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B118" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="C118" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D118" s="6" t="s">
         <v>206</v>
-      </c>
-      <c r="C118" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D118" s="6" t="s">
-        <v>207</v>
       </c>
       <c r="E118" s="5">
         <v>1520</v>
@@ -4888,22 +4903,22 @@
       <c r="H118" s="5">
         <v>3</v>
       </c>
-      <c r="I118" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I118" s="11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B119" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="C119" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D119" s="6" t="s">
         <v>219</v>
-      </c>
-      <c r="C119" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D119" s="6" t="s">
-        <v>220</v>
       </c>
       <c r="E119" s="5">
         <v>1525</v>
@@ -4917,22 +4932,22 @@
       <c r="H119" s="5">
         <v>3</v>
       </c>
-      <c r="I119" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I119" s="11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B120" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="B120" s="4" t="s">
-        <v>211</v>
-      </c>
       <c r="C120" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E120" s="5">
         <v>1525</v>
@@ -4946,11 +4961,11 @@
       <c r="H120" s="5">
         <v>3</v>
       </c>
-      <c r="I120" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I120" s="11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="4" t="s">
         <v>155</v>
       </c>
@@ -4975,11 +4990,11 @@
       <c r="H121" s="5">
         <v>3</v>
       </c>
-      <c r="I121" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I121" s="11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="s">
         <v>124</v>
       </c>
@@ -4999,16 +5014,16 @@
         <v>3</v>
       </c>
       <c r="G122" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H122" s="5">
         <v>2</v>
       </c>
-      <c r="I122" s="5">
+      <c r="I122" s="11">
         <v>561349000</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="s">
         <v>115</v>
       </c>
@@ -5028,16 +5043,16 @@
         <v>3</v>
       </c>
       <c r="G123" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H123" s="5">
         <v>2</v>
       </c>
-      <c r="I123" s="5">
+      <c r="I123" s="11">
         <v>561349000</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A124" s="4" t="s">
         <v>56</v>
       </c>
@@ -5057,16 +5072,16 @@
         <v>3</v>
       </c>
       <c r="G124" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H124" s="5">
         <v>2</v>
       </c>
-      <c r="I124" s="5">
+      <c r="I124" s="11">
         <v>561349000</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="4" t="s">
         <v>54</v>
       </c>
@@ -5086,27 +5101,27 @@
         <v>3</v>
       </c>
       <c r="G125" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H125" s="5">
         <v>2</v>
       </c>
-      <c r="I125" s="5">
+      <c r="I125" s="11">
         <v>561349000</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B126" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="B126" s="4" t="s">
+      <c r="C126" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D126" s="6" t="s">
         <v>223</v>
-      </c>
-      <c r="C126" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D126" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="E126" s="5">
         <v>1100</v>
@@ -5115,27 +5130,27 @@
         <v>3</v>
       </c>
       <c r="G126" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H126" s="5">
         <v>2</v>
       </c>
-      <c r="I126" s="5">
+      <c r="I126" s="11">
         <v>561349000</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="B127" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="C127" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D127" s="6" t="s">
         <v>226</v>
-      </c>
-      <c r="C127" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D127" s="6" t="s">
-        <v>227</v>
       </c>
       <c r="E127" s="5">
         <v>1100</v>
@@ -5144,16 +5159,16 @@
         <v>3</v>
       </c>
       <c r="G127" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H127" s="5">
         <v>2</v>
       </c>
-      <c r="I127" s="5">
+      <c r="I127" s="11">
         <v>561349000</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="4" t="s">
         <v>14</v>
       </c>
@@ -5178,11 +5193,11 @@
       <c r="H128" s="5">
         <v>7</v>
       </c>
-      <c r="I128" s="5" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I128" s="11" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="4" t="s">
         <v>14</v>
       </c>
@@ -5202,16 +5217,16 @@
         <v>3</v>
       </c>
       <c r="G129" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H129" s="5">
         <v>7</v>
       </c>
-      <c r="I129" s="5" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I129" s="11" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="4" t="s">
         <v>14</v>
       </c>
@@ -5231,16 +5246,16 @@
         <v>3</v>
       </c>
       <c r="G130" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H130" s="5">
         <v>7</v>
       </c>
-      <c r="I130" s="5" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I130" s="11" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A131" s="4" t="s">
         <v>115</v>
       </c>
@@ -5265,8 +5280,8 @@
       <c r="H131" s="5">
         <v>7</v>
       </c>
-      <c r="I131" s="5" t="s">
-        <v>230</v>
+      <c r="I131" s="11" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5294,11 +5309,11 @@
       <c r="H132" s="5">
         <v>7</v>
       </c>
-      <c r="I132" s="5" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I132" s="11" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A133" s="4" t="s">
         <v>112</v>
       </c>
@@ -5318,16 +5333,16 @@
         <v>7</v>
       </c>
       <c r="G133" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H133" s="5">
         <v>7</v>
       </c>
-      <c r="I133" s="5" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I133" s="11" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A134" s="4" t="s">
         <v>115</v>
       </c>
@@ -5347,16 +5362,16 @@
         <v>7</v>
       </c>
       <c r="G134" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H134" s="5">
         <v>7</v>
       </c>
-      <c r="I134" s="5" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I134" s="11" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A135" s="4" t="s">
         <v>54</v>
       </c>
@@ -5367,7 +5382,7 @@
         <v>51</v>
       </c>
       <c r="D135" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E135" s="5">
         <v>1810</v>
@@ -5381,7 +5396,7 @@
       <c r="H135" s="5">
         <v>3</v>
       </c>
-      <c r="I135" s="5" t="s">
+      <c r="I135" s="11" t="s">
         <v>123</v>
       </c>
     </row>
@@ -5410,8 +5425,8 @@
       <c r="H136" s="5">
         <v>7</v>
       </c>
-      <c r="I136" s="5" t="s">
-        <v>237</v>
+      <c r="I136" s="11" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="137" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5439,8 +5454,8 @@
       <c r="H137" s="5">
         <v>7</v>
       </c>
-      <c r="I137" s="5" t="s">
-        <v>238</v>
+      <c r="I137" s="11" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5468,11 +5483,11 @@
       <c r="H138" s="5">
         <v>7</v>
       </c>
-      <c r="I138" s="5" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I138" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A139" s="4" t="s">
         <v>64</v>
       </c>
@@ -5498,11 +5513,11 @@
       <c r="H139" s="5">
         <v>3</v>
       </c>
-      <c r="I139" s="5" t="s">
+      <c r="I139" s="11" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A140" s="4" t="s">
         <v>35</v>
       </c>
@@ -5513,7 +5528,7 @@
         <v>129</v>
       </c>
       <c r="D140" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E140" s="5">
         <v>360</v>
@@ -5527,11 +5542,11 @@
       <c r="H140" s="5">
         <v>11</v>
       </c>
-      <c r="I140" s="5" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I140" s="11" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="4" t="s">
         <v>54</v>
       </c>
@@ -5542,7 +5557,7 @@
         <v>51</v>
       </c>
       <c r="D141" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E141" s="5">
         <v>2020</v>
@@ -5556,11 +5571,11 @@
       <c r="H141" s="5">
         <v>3</v>
       </c>
-      <c r="I141" s="5" t="s">
+      <c r="I141" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="142" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A142" s="4" t="s">
         <v>8</v>
       </c>
@@ -5571,7 +5586,7 @@
         <v>51</v>
       </c>
       <c r="D142" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E142" s="5">
         <v>1825</v>
@@ -5585,11 +5600,11 @@
       <c r="H142" s="5">
         <v>3</v>
       </c>
-      <c r="I142" s="5" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I142" s="11" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A143" s="4" t="s">
         <v>14</v>
       </c>
@@ -5600,7 +5615,7 @@
         <v>51</v>
       </c>
       <c r="D143" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E143" s="5">
         <v>1825</v>
@@ -5614,11 +5629,11 @@
       <c r="H143" s="5">
         <v>3</v>
       </c>
-      <c r="I143" s="5" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="144" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I143" s="11" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A144" s="4" t="s">
         <v>59</v>
       </c>
@@ -5643,22 +5658,22 @@
       <c r="H144" s="5">
         <v>3</v>
       </c>
-      <c r="I144" s="5" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I144" s="11" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A145" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B145" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="B145" s="4" t="s">
-        <v>202</v>
-      </c>
       <c r="C145" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D145" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E145" s="5">
         <v>1825</v>
@@ -5672,11 +5687,11 @@
       <c r="H145" s="5">
         <v>3</v>
       </c>
-      <c r="I145" s="5" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="146" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I145" s="11" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A146" s="4" t="s">
         <v>8</v>
       </c>
@@ -5687,7 +5702,7 @@
         <v>51</v>
       </c>
       <c r="D146" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E146" s="5">
         <f>2400+10</f>
@@ -5697,27 +5712,27 @@
         <v>3</v>
       </c>
       <c r="G146" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H146" s="5">
         <v>2</v>
       </c>
-      <c r="I146" s="5">
+      <c r="I146" s="11">
         <v>561349000</v>
       </c>
     </row>
-    <row r="147" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A147" s="4" t="s">
         <v>155</v>
       </c>
       <c r="B147" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="C147" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D147" s="6" t="s">
         <v>246</v>
-      </c>
-      <c r="C147" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D147" s="6" t="s">
-        <v>247</v>
       </c>
       <c r="E147" s="5">
         <f>2400+10</f>
@@ -5727,16 +5742,16 @@
         <v>3</v>
       </c>
       <c r="G147" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H147" s="5">
         <v>2</v>
       </c>
-      <c r="I147" s="5">
+      <c r="I147" s="11">
         <v>561349000</v>
       </c>
     </row>
-    <row r="148" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A148" s="4" t="s">
         <v>145</v>
       </c>
@@ -5747,7 +5762,7 @@
         <v>51</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E148" s="5">
         <f>2400+10</f>
@@ -5762,11 +5777,11 @@
       <c r="H148" s="5">
         <v>3</v>
       </c>
-      <c r="I148" s="5" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="149" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I148" s="11" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A149" s="4" t="s">
         <v>17</v>
       </c>
@@ -5777,7 +5792,7 @@
         <v>51</v>
       </c>
       <c r="D149" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E149" s="5">
         <f>2400+10</f>
@@ -5792,11 +5807,11 @@
       <c r="H149" s="5">
         <v>3</v>
       </c>
-      <c r="I149" s="5" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="150" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I149" s="11" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A150" s="4" t="s">
         <v>54</v>
       </c>
@@ -5807,7 +5822,7 @@
         <v>51</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E150" s="5">
         <f>1060+35</f>
@@ -5817,27 +5832,27 @@
         <v>3</v>
       </c>
       <c r="G150" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H150" s="5">
         <v>7</v>
       </c>
-      <c r="I150" s="5" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="151" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I150" s="11" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A151" s="4" t="s">
         <v>115</v>
       </c>
       <c r="B151" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="C151" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D151" s="6" t="s">
         <v>251</v>
-      </c>
-      <c r="C151" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D151" s="6" t="s">
-        <v>252</v>
       </c>
       <c r="E151" s="5">
         <f>1840+5</f>
@@ -5847,16 +5862,16 @@
         <v>3</v>
       </c>
       <c r="G151" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H151" s="5">
         <v>2</v>
       </c>
-      <c r="I151" s="5">
+      <c r="I151" s="11">
         <v>561349000</v>
       </c>
     </row>
-    <row r="152" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A152" s="4" t="s">
         <v>59</v>
       </c>
@@ -5882,22 +5897,22 @@
       <c r="H152" s="5">
         <v>3</v>
       </c>
-      <c r="I152" s="5" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="153" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I152" s="11" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A153" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B153" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C153" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D153" s="6" t="s">
         <v>253</v>
-      </c>
-      <c r="C153" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D153" s="6" t="s">
-        <v>254</v>
       </c>
       <c r="E153" s="5">
         <f>1650+35</f>
@@ -5907,27 +5922,27 @@
         <v>3</v>
       </c>
       <c r="G153" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H153" s="5">
         <v>2</v>
       </c>
-      <c r="I153" s="5" t="s">
+      <c r="I153" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="154" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A154" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B154" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C154" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D154" s="6" t="s">
         <v>255</v>
-      </c>
-      <c r="C154" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D154" s="6" t="s">
-        <v>256</v>
       </c>
       <c r="E154" s="5">
         <f>1650+35</f>
@@ -5937,16 +5952,16 @@
         <v>3</v>
       </c>
       <c r="G154" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H154" s="5">
         <v>2</v>
       </c>
-      <c r="I154" s="5" t="s">
+      <c r="I154" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="155" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A155" s="4" t="s">
         <v>17</v>
       </c>
@@ -5957,7 +5972,7 @@
         <v>51</v>
       </c>
       <c r="D155" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E155" s="5">
         <v>3130</v>
@@ -5971,11 +5986,11 @@
       <c r="H155" s="5">
         <v>3</v>
       </c>
-      <c r="I155" s="5" t="s">
+      <c r="I155" s="11" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="156" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A156" s="4" t="s">
         <v>54</v>
       </c>
@@ -5986,7 +6001,7 @@
         <v>51</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E156" s="5">
         <f>4680+50</f>
@@ -6001,11 +6016,11 @@
       <c r="H156" s="5">
         <v>3</v>
       </c>
-      <c r="I156" s="5" t="s">
+      <c r="I156" s="11" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="157" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A157" s="4" t="s">
         <v>59</v>
       </c>
@@ -6031,11 +6046,11 @@
       <c r="H157" s="5">
         <v>2</v>
       </c>
-      <c r="I157" s="5" t="s">
+      <c r="I157" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A158" s="4" t="s">
         <v>84</v>
       </c>
@@ -6060,11 +6075,11 @@
       <c r="H158" s="5">
         <v>4.8</v>
       </c>
-      <c r="I158" s="5" t="s">
+      <c r="I158" s="11" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="159" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A159" s="4" t="s">
         <v>68</v>
       </c>
@@ -6089,11 +6104,11 @@
       <c r="H159" s="5">
         <v>4.8</v>
       </c>
-      <c r="I159" s="5" t="s">
+      <c r="I159" s="11" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="160" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A160" s="4" t="s">
         <v>54</v>
       </c>
@@ -6118,11 +6133,11 @@
       <c r="H160" s="5">
         <v>3.5</v>
       </c>
-      <c r="I160" s="5" t="s">
+      <c r="I160" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="161" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A161" s="4" t="s">
         <v>64</v>
       </c>
@@ -6148,11 +6163,11 @@
       <c r="H161" s="5">
         <v>7</v>
       </c>
-      <c r="I161" s="5" t="s">
+      <c r="I161" s="11" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="162" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A162" s="4" t="s">
         <v>64</v>
       </c>
@@ -6177,11 +6192,11 @@
       <c r="H162" s="5">
         <v>7</v>
       </c>
-      <c r="I162" s="5" t="s">
+      <c r="I162" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="163" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A163" s="4" t="s">
         <v>64</v>
       </c>
@@ -6207,11 +6222,11 @@
       <c r="H163" s="5">
         <v>7</v>
       </c>
-      <c r="I163" s="5" t="s">
+      <c r="I163" s="11" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="164" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A164" s="4" t="s">
         <v>92</v>
       </c>
@@ -6236,11 +6251,11 @@
       <c r="H164" s="5">
         <v>7</v>
       </c>
-      <c r="I164" s="5" t="s">
+      <c r="I164" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="165" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A165" s="4" t="s">
         <v>92</v>
       </c>
@@ -6266,11 +6281,11 @@
       <c r="H165" s="5">
         <v>7</v>
       </c>
-      <c r="I165" s="5" t="s">
+      <c r="I165" s="11" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="166" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A166" s="4" t="s">
         <v>92</v>
       </c>
@@ -6295,11 +6310,11 @@
       <c r="H166" s="5">
         <v>7</v>
       </c>
-      <c r="I166" s="5" t="s">
+      <c r="I166" s="11" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="167" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A167" s="4" t="s">
         <v>49</v>
       </c>
@@ -6324,11 +6339,11 @@
       <c r="H167" s="5">
         <v>3.5</v>
       </c>
-      <c r="I167" s="5" t="s">
+      <c r="I167" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="168" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A168" s="4" t="s">
         <v>14</v>
       </c>
@@ -6353,11 +6368,11 @@
       <c r="H168" s="5">
         <v>3</v>
       </c>
-      <c r="I168" s="5" t="s">
+      <c r="I168" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A169" s="4" t="s">
         <v>98</v>
       </c>
@@ -6382,11 +6397,11 @@
       <c r="H169" s="5">
         <v>11</v>
       </c>
-      <c r="I169" s="5" t="s">
+      <c r="I169" s="11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="170" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A170" s="4" t="s">
         <v>98</v>
       </c>
@@ -6411,11 +6426,11 @@
       <c r="H170" s="5">
         <v>11</v>
       </c>
-      <c r="I170" s="5" t="s">
+      <c r="I170" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="171" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A171" s="4" t="s">
         <v>98</v>
       </c>
@@ -6441,11 +6456,11 @@
       <c r="H171" s="5">
         <v>11</v>
       </c>
-      <c r="I171" s="5" t="s">
+      <c r="I171" s="11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="172" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A172" s="4" t="s">
         <v>107</v>
       </c>
@@ -6471,11 +6486,11 @@
       <c r="H172" s="5">
         <v>7</v>
       </c>
-      <c r="I172" s="5" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="173" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I172" s="11" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A173" s="4" t="s">
         <v>54</v>
       </c>
@@ -6501,11 +6516,11 @@
       <c r="H173" s="5">
         <v>7</v>
       </c>
-      <c r="I173" s="5" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="174" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I173" s="11" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A174" s="4" t="s">
         <v>14</v>
       </c>
@@ -6530,11 +6545,11 @@
       <c r="H174" s="5">
         <v>3</v>
       </c>
-      <c r="I174" s="5" t="s">
+      <c r="I174" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="175" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A175" s="4" t="s">
         <v>112</v>
       </c>
@@ -6559,11 +6574,11 @@
       <c r="H175" s="5">
         <v>3</v>
       </c>
-      <c r="I175" s="5" t="s">
+      <c r="I175" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="176" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A176" s="4" t="s">
         <v>115</v>
       </c>
@@ -6589,11 +6604,11 @@
       <c r="H176" s="5">
         <v>7</v>
       </c>
-      <c r="I176" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="177" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I176" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A177" s="4" t="s">
         <v>112</v>
       </c>
@@ -6619,11 +6634,11 @@
       <c r="H177" s="5">
         <v>7</v>
       </c>
-      <c r="I177" s="5" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="178" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I177" s="11" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A178" s="4" t="s">
         <v>119</v>
       </c>
@@ -6648,11 +6663,11 @@
       <c r="H178" s="5">
         <v>3</v>
       </c>
-      <c r="I178" s="5" t="s">
+      <c r="I178" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="179" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A179" s="4" t="s">
         <v>49</v>
       </c>
@@ -6677,11 +6692,11 @@
       <c r="H179" s="5">
         <v>3</v>
       </c>
-      <c r="I179" s="5" t="s">
+      <c r="I179" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="180" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A180" s="4" t="s">
         <v>8</v>
       </c>
@@ -6692,7 +6707,7 @@
         <v>51</v>
       </c>
       <c r="D180" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E180" s="5">
         <v>1045</v>
@@ -6706,22 +6721,22 @@
       <c r="H180" s="5">
         <v>2</v>
       </c>
-      <c r="I180" s="5">
+      <c r="I180" s="11">
         <v>561349001</v>
       </c>
     </row>
-    <row r="181" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A181" s="4" t="s">
         <v>155</v>
       </c>
       <c r="B181" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C181" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D181" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E181" s="5">
         <v>1045</v>
@@ -6735,11 +6750,11 @@
       <c r="H181" s="5">
         <v>2</v>
       </c>
-      <c r="I181" s="5">
+      <c r="I181" s="11">
         <v>561349001</v>
       </c>
     </row>
-    <row r="182" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A182" s="4" t="s">
         <v>145</v>
       </c>
@@ -6764,11 +6779,11 @@
       <c r="H182" s="5">
         <v>7</v>
       </c>
-      <c r="I182" s="5" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="183" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I182" s="11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A183" s="4" t="s">
         <v>92</v>
       </c>
@@ -6793,11 +6808,11 @@
       <c r="H183" s="5">
         <v>7</v>
       </c>
-      <c r="I183" s="5" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="184" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I183" s="11" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A184" s="4" t="s">
         <v>145</v>
       </c>
@@ -6817,16 +6832,16 @@
         <v>3</v>
       </c>
       <c r="G184" s="11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H184" s="5">
         <v>7</v>
       </c>
-      <c r="I184" s="5" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="185" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I184" s="11" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A185" s="4" t="s">
         <v>119</v>
       </c>
@@ -6846,16 +6861,16 @@
         <v>3</v>
       </c>
       <c r="G185" s="11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H185" s="5">
         <v>3.5</v>
       </c>
-      <c r="I185" s="5" t="s">
+      <c r="I185" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="186" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A186" s="4" t="s">
         <v>8</v>
       </c>
@@ -6880,11 +6895,11 @@
       <c r="H186" s="5">
         <v>3</v>
       </c>
-      <c r="I186" s="5" t="s">
+      <c r="I186" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="187" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A187" s="4" t="s">
         <v>14</v>
       </c>
@@ -6909,11 +6924,11 @@
       <c r="H187" s="5">
         <v>3</v>
       </c>
-      <c r="I187" s="5" t="s">
+      <c r="I187" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="188" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A188" s="4" t="s">
         <v>17</v>
       </c>
@@ -6938,11 +6953,11 @@
       <c r="H188" s="5">
         <v>3</v>
       </c>
-      <c r="I188" s="5" t="s">
+      <c r="I188" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="189" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A189" s="4" t="s">
         <v>133</v>
       </c>
@@ -6967,22 +6982,22 @@
       <c r="H189" s="5">
         <v>4.8</v>
       </c>
-      <c r="I189" s="5" t="s">
+      <c r="I189" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A190" s="4" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="190" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A190" s="4" t="s">
+      <c r="B190" s="4" t="s">
         <v>267</v>
-      </c>
-      <c r="B190" s="4" t="s">
-        <v>268</v>
       </c>
       <c r="C190" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D190" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E190" s="5">
         <v>185</v>
@@ -6996,11 +7011,11 @@
       <c r="H190" s="5">
         <v>4.8</v>
       </c>
-      <c r="I190" s="5" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="191" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I190" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A191" s="4" t="s">
         <v>21</v>
       </c>
@@ -7025,11 +7040,11 @@
       <c r="H191" s="5">
         <v>3.5</v>
       </c>
-      <c r="I191" s="5" t="s">
+      <c r="I191" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="192" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A192" s="4" t="s">
         <v>27</v>
       </c>
@@ -7054,11 +7069,11 @@
       <c r="H192" s="5">
         <v>3.5</v>
       </c>
-      <c r="I192" s="5" t="s">
+      <c r="I192" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="193" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A193" s="4" t="s">
         <v>30</v>
       </c>
@@ -7083,11 +7098,11 @@
       <c r="H193" s="5">
         <v>3.5</v>
       </c>
-      <c r="I193" s="5" t="s">
+      <c r="I193" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A194" s="4" t="s">
         <v>33</v>
       </c>
@@ -7112,11 +7127,11 @@
       <c r="H194" s="5">
         <v>3.5</v>
       </c>
-      <c r="I194" s="5" t="s">
+      <c r="I194" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="195" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A195" s="4" t="s">
         <v>35</v>
       </c>
@@ -7124,7 +7139,7 @@
         <v>36</v>
       </c>
       <c r="C195" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D195" s="6" t="s">
         <v>38</v>
@@ -7141,11 +7156,11 @@
       <c r="H195" s="5">
         <v>3.5</v>
       </c>
-      <c r="I195" s="5" t="s">
+      <c r="I195" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A196" s="4" t="s">
         <v>35</v>
       </c>
@@ -7153,7 +7168,7 @@
         <v>36</v>
       </c>
       <c r="C196" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D196" s="6" t="s">
         <v>38</v>
@@ -7168,11 +7183,11 @@
       <c r="H196" s="5">
         <v>5</v>
       </c>
-      <c r="I196" s="5" t="s">
+      <c r="I196" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="197" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A197" s="4" t="s">
         <v>41</v>
       </c>
@@ -7197,11 +7212,11 @@
       <c r="H197" s="5">
         <v>5</v>
       </c>
-      <c r="I197" s="5" t="s">
+      <c r="I197" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="198" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A198" s="4" t="s">
         <v>45</v>
       </c>
@@ -7226,11 +7241,11 @@
       <c r="H198" s="5">
         <v>5</v>
       </c>
-      <c r="I198" s="5" t="s">
+      <c r="I198" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="199" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A199" s="4" t="s">
         <v>8</v>
       </c>
@@ -7255,11 +7270,11 @@
       <c r="H199" s="5">
         <v>3</v>
       </c>
-      <c r="I199" s="5" t="s">
+      <c r="I199" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="200" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A200" s="4" t="s">
         <v>14</v>
       </c>
@@ -7284,11 +7299,11 @@
       <c r="H200" s="5">
         <v>3</v>
       </c>
-      <c r="I200" s="5" t="s">
+      <c r="I200" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="201" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A201" s="4" t="s">
         <v>17</v>
       </c>
@@ -7313,11 +7328,11 @@
       <c r="H201" s="5">
         <v>3</v>
       </c>
-      <c r="I201" s="5" t="s">
+      <c r="I201" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="202" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A202" s="4" t="s">
         <v>21</v>
       </c>
@@ -7342,11 +7357,11 @@
       <c r="H202" s="5">
         <v>3.5</v>
       </c>
-      <c r="I202" s="5" t="s">
+      <c r="I202" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="203" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A203" s="4" t="s">
         <v>27</v>
       </c>
@@ -7371,11 +7386,11 @@
       <c r="H203" s="5">
         <v>3.5</v>
       </c>
-      <c r="I203" s="5" t="s">
+      <c r="I203" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="204" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A204" s="4" t="s">
         <v>30</v>
       </c>
@@ -7400,11 +7415,11 @@
       <c r="H204" s="5">
         <v>3.5</v>
       </c>
-      <c r="I204" s="5" t="s">
+      <c r="I204" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="205" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A205" s="4" t="s">
         <v>33</v>
       </c>
@@ -7429,11 +7444,11 @@
       <c r="H205" s="5">
         <v>3.5</v>
       </c>
-      <c r="I205" s="5" t="s">
+      <c r="I205" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="206" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A206" s="4" t="s">
         <v>35</v>
       </c>
@@ -7458,11 +7473,11 @@
       <c r="H206" s="5">
         <v>3.5</v>
       </c>
-      <c r="I206" s="5" t="s">
+      <c r="I206" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="207" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A207" s="4" t="s">
         <v>35</v>
       </c>
@@ -7485,11 +7500,11 @@
       <c r="H207" s="5">
         <v>5</v>
       </c>
-      <c r="I207" s="5" t="s">
+      <c r="I207" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="208" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A208" s="4" t="s">
         <v>41</v>
       </c>
@@ -7514,11 +7529,11 @@
       <c r="H208" s="5">
         <v>5</v>
       </c>
-      <c r="I208" s="5" t="s">
+      <c r="I208" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:9" ht="15.6" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A209" s="4" t="s">
         <v>45</v>
       </c>
@@ -7543,12 +7558,19 @@
       <c r="H209" s="5">
         <v>5</v>
       </c>
-      <c r="I209" s="5" t="s">
+      <c r="I209" s="11" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="210" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <autoFilter ref="A1:I209" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="39000048"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>